<commit_message>
Started work on the board
</commit_message>
<xml_diff>
--- a/Flight Stick Information.xlsx
+++ b/Flight Stick Information.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22607"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thete\FlightStick\Virtual-Pilot-XInput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A7EB758-BD40-417A-B9AE-155679DB4E70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54072A08-29F9-4156-87EC-76F4B40C93DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{1C55DCC2-B92B-40E3-A31E-8283370B0490}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="60" windowWidth="28800" windowHeight="15555" xr2:uid="{1C55DCC2-B92B-40E3-A31E-8283370B0490}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="123">
   <si>
     <t>X1</t>
   </si>
@@ -395,13 +395,13 @@
     <t>Breadboard Connection</t>
   </si>
   <si>
-    <t>A6</t>
-  </si>
-  <si>
-    <t>A5</t>
-  </si>
-  <si>
-    <t>A4</t>
+    <t>a5</t>
+  </si>
+  <si>
+    <t>a4</t>
+  </si>
+  <si>
+    <t>a3</t>
   </si>
 </sst>
 </file>
@@ -441,7 +441,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -467,13 +467,75 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -488,6 +550,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -511,13 +579,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>200025</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>523875</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
@@ -571,13 +639,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>722086</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
@@ -638,13 +706,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>790575</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>26761</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
@@ -705,13 +773,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>512536</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
@@ -772,13 +840,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>436336</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
@@ -843,13 +911,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>723900</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>1141186</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
@@ -910,13 +978,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>645886</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -977,13 +1045,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>666750</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>1084036</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
@@ -1044,13 +1112,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>1028700</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>264886</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -1111,7 +1179,7 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>95251</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
@@ -1471,10 +1539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA414539-3720-4AA2-BB48-D154F2256BF9}">
-  <dimension ref="A1:AA40"/>
+  <dimension ref="A1:AB40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1482,17 +1550,19 @@
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="6" width="38" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>119</v>
       </c>
@@ -1502,14 +1572,17 @@
       <c r="E1" t="s">
         <v>27</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11</v>
       </c>
@@ -1522,20 +1595,21 @@
       <c r="E2" t="s">
         <v>35</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="8"/>
+      <c r="G2" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>36</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>5</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1548,20 +1622,23 @@
       <c r="E3" t="s">
         <v>31</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="8">
+        <v>6</v>
+      </c>
+      <c r="G3" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>3</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>6</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1574,20 +1651,23 @@
       <c r="E4" t="s">
         <v>32</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="8">
+        <v>5</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>4</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>16</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1600,36 +1680,39 @@
       <c r="E5" t="s">
         <v>23</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="8">
+        <v>4</v>
+      </c>
+      <c r="G5" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>8</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>20</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="P5" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
       <c r="U5" s="2"/>
       <c r="V5" s="2"/>
-      <c r="X5" s="2" t="s">
+      <c r="W5" s="2"/>
+      <c r="Y5" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
       <c r="AA5" s="2"/>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB5" s="2"/>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1642,42 +1725,45 @@
       <c r="E6" t="s">
         <v>23</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="8">
+        <v>3</v>
+      </c>
+      <c r="G6" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="I6" t="s">
+      <c r="H6" s="2"/>
+      <c r="J6" t="s">
         <v>9</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>20</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>41</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>42</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>43</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>45</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>44</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>46</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>47</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1690,26 +1776,29 @@
       <c r="E7" t="s">
         <v>23</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="8">
+        <v>2</v>
+      </c>
+      <c r="G7" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="I7" t="s">
+      <c r="H7" s="2"/>
+      <c r="J7" t="s">
         <v>10</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>21</v>
       </c>
-      <c r="P7" s="2" t="s">
+      <c r="Q7" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
       <c r="U7" s="2"/>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="V7" s="2"/>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1722,44 +1811,49 @@
       <c r="E8" t="s">
         <v>23</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="8">
+        <v>1</v>
+      </c>
+      <c r="G8" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="I8" t="s">
+      <c r="H8" s="2"/>
+      <c r="J8" t="s">
         <v>14</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>20</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>41</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="R8" t="s">
         <v>42</v>
       </c>
-      <c r="R8" t="s">
+      <c r="S8" t="s">
         <v>52</v>
       </c>
-      <c r="S8" t="s">
+      <c r="T8" t="s">
         <v>51</v>
       </c>
-      <c r="T8" t="s">
+      <c r="U8" t="s">
         <v>25</v>
       </c>
-      <c r="U8" t="s">
+      <c r="V8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="I9" t="s">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="F9" s="8"/>
+      <c r="G9" s="9"/>
+      <c r="J9" t="s">
         <v>15</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1775,11 +1869,14 @@
       <c r="E10" t="s">
         <v>30</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="8">
+        <v>18</v>
+      </c>
+      <c r="G10" s="9" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1795,14 +1892,17 @@
       <c r="E11" t="s">
         <v>26</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="8">
+        <v>17</v>
+      </c>
+      <c r="G11" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1818,14 +1918,17 @@
       <c r="E12" t="s">
         <v>23</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="8">
+        <v>16</v>
+      </c>
+      <c r="G12" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1841,14 +1944,17 @@
       <c r="E13" t="s">
         <v>31</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="8">
+        <v>15</v>
+      </c>
+      <c r="G13" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1864,14 +1970,17 @@
       <c r="E14" t="s">
         <v>32</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="8">
+        <v>14</v>
+      </c>
+      <c r="G14" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1887,14 +1996,17 @@
       <c r="E15" t="s">
         <v>25</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="8">
+        <v>13</v>
+      </c>
+      <c r="G15" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1910,14 +2022,17 @@
       <c r="E16" t="s">
         <v>23</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="8">
+        <v>12</v>
+      </c>
+      <c r="G16" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="H16" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1933,12 +2048,15 @@
       <c r="E17" t="s">
         <v>23</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="8">
+        <v>11</v>
+      </c>
+      <c r="G17" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -1954,12 +2072,15 @@
       <c r="E18" t="s">
         <v>23</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="8">
+        <v>10</v>
+      </c>
+      <c r="G18" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -1975,14 +2096,17 @@
       <c r="E19" t="s">
         <v>31</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="8">
+        <v>9</v>
+      </c>
+      <c r="G19" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -1998,14 +2122,21 @@
       <c r="E20" t="s">
         <v>32</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="8">
+        <v>8</v>
+      </c>
+      <c r="G20" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="F21" s="8"/>
+      <c r="G21" s="9"/>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -2015,26 +2146,26 @@
       <c r="E22" t="s">
         <v>40</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="10"/>
+      <c r="G22" s="11" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>65</v>
       </c>
       <c r="C25" t="s">
         <v>65</v>
       </c>
-      <c r="N25" s="4" t="s">
+      <c r="O25" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="O25" s="4"/>
       <c r="P25" s="4"/>
       <c r="Q25" s="4"/>
       <c r="R25" s="4"/>
@@ -2042,19 +2173,19 @@
       <c r="T25" s="4"/>
       <c r="U25" s="4"/>
       <c r="V25" s="4"/>
-    </row>
-    <row r="26" spans="1:22" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W25" s="4"/>
+    </row>
+    <row r="26" spans="1:23" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>117</v>
       </c>
       <c r="C26" t="s">
         <v>8</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="H26" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H26" s="2"/>
-      <c r="N26" s="5"/>
+      <c r="I26" s="2"/>
       <c r="O26" s="5"/>
       <c r="P26" s="5"/>
       <c r="Q26" s="5"/>
@@ -2063,8 +2194,9 @@
       <c r="T26" s="5"/>
       <c r="U26" s="5"/>
       <c r="V26" s="5"/>
-    </row>
-    <row r="27" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="W26" s="5"/>
+    </row>
+    <row r="27" spans="1:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>64</v>
       </c>
@@ -2072,211 +2204,211 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="R28" s="3" t="s">
+    <row r="28" spans="1:23" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S28" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="S28" s="3"/>
-      <c r="U28" s="3" t="s">
+      <c r="T28" s="3"/>
+      <c r="V28" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="V28" s="3"/>
-    </row>
-    <row r="29" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="W28" s="3"/>
+    </row>
+    <row r="29" spans="1:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>63</v>
       </c>
-      <c r="N29" t="s">
+      <c r="O29" t="s">
         <v>57</v>
       </c>
-      <c r="O29" t="s">
+      <c r="P29" t="s">
         <v>60</v>
       </c>
-      <c r="R29" t="s">
+      <c r="S29" t="s">
         <v>60</v>
       </c>
-      <c r="S29" t="s">
+      <c r="T29" t="s">
         <v>86</v>
       </c>
-      <c r="U29" t="s">
+      <c r="V29" t="s">
         <v>59</v>
       </c>
-      <c r="V29" t="s">
+      <c r="W29" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>65</v>
       </c>
       <c r="C30" t="s">
         <v>118</v>
       </c>
-      <c r="N30" t="s">
+      <c r="O30" t="s">
         <v>58</v>
       </c>
-      <c r="O30" t="s">
+      <c r="P30" t="s">
         <v>69</v>
       </c>
-      <c r="R30" t="s">
+      <c r="S30" t="s">
         <v>72</v>
       </c>
-      <c r="S30" t="s">
+      <c r="T30" t="s">
         <v>86</v>
       </c>
-      <c r="U30" t="s">
+      <c r="V30" t="s">
         <v>81</v>
       </c>
-      <c r="V30" t="s">
+      <c r="W30" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>117</v>
       </c>
       <c r="C31" t="s">
         <v>9</v>
       </c>
-      <c r="R31" t="s">
+      <c r="S31" t="s">
         <v>65</v>
       </c>
-      <c r="S31" t="s">
+      <c r="T31" t="s">
         <v>80</v>
       </c>
-      <c r="U31" t="s">
+      <c r="V31" t="s">
         <v>65</v>
       </c>
-      <c r="V31" t="s">
+      <c r="W31" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>64</v>
       </c>
       <c r="C32" t="s">
         <v>64</v>
       </c>
-      <c r="N32" t="s">
+      <c r="O32" t="s">
         <v>67</v>
       </c>
-      <c r="O32" t="s">
+      <c r="P32" t="s">
         <v>59</v>
       </c>
-      <c r="R32" t="s">
+      <c r="S32" t="s">
         <v>73</v>
       </c>
-      <c r="S32" t="s">
+      <c r="T32" t="s">
         <v>80</v>
       </c>
-      <c r="U32" t="s">
+      <c r="V32" t="s">
         <v>76</v>
       </c>
-      <c r="V32" t="s">
+      <c r="W32" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="33" spans="14:22" x14ac:dyDescent="0.25">
-      <c r="N33" t="s">
+    <row r="33" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="O33" t="s">
         <v>68</v>
       </c>
-      <c r="O33" t="s">
+      <c r="P33" t="s">
         <v>70</v>
       </c>
-      <c r="U33" t="s">
+      <c r="V33" t="s">
         <v>82</v>
       </c>
-      <c r="V33" t="s">
+      <c r="W33" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="35" spans="14:22" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="N35" t="s">
+    <row r="35" spans="15:23" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="O35" t="s">
         <v>61</v>
       </c>
-      <c r="O35" t="s">
+      <c r="P35" t="s">
         <v>62</v>
       </c>
-      <c r="R35" s="3" t="s">
+      <c r="S35" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="S35" s="3"/>
-    </row>
-    <row r="36" spans="14:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="N36" t="s">
+      <c r="T35" s="3"/>
+    </row>
+    <row r="36" spans="15:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="O36" t="s">
         <v>8</v>
       </c>
-      <c r="O36" t="s">
+      <c r="P36" t="s">
         <v>41</v>
       </c>
-      <c r="R36" t="s">
+      <c r="S36" t="s">
         <v>79</v>
       </c>
-      <c r="S36" t="s">
+      <c r="T36" t="s">
         <v>85</v>
       </c>
-      <c r="U36" s="1"/>
       <c r="V36" s="1"/>
-    </row>
-    <row r="37" spans="14:22" x14ac:dyDescent="0.25">
-      <c r="N37" t="s">
+      <c r="W36" s="1"/>
+    </row>
+    <row r="37" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="O37" t="s">
         <v>9</v>
       </c>
-      <c r="O37" t="s">
+      <c r="P37" t="s">
         <v>63</v>
       </c>
-      <c r="R37" t="s">
+      <c r="S37" t="s">
         <v>65</v>
       </c>
-      <c r="S37" t="s">
+      <c r="T37" t="s">
         <v>75</v>
       </c>
-      <c r="U37" s="1"/>
       <c r="V37" s="1"/>
-    </row>
-    <row r="38" spans="14:22" x14ac:dyDescent="0.25">
-      <c r="R38" t="s">
+      <c r="W37" s="1"/>
+    </row>
+    <row r="38" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="S38" t="s">
         <v>25</v>
       </c>
-      <c r="S38" t="s">
+      <c r="T38" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="14:22" x14ac:dyDescent="0.25">
-      <c r="N39" t="s">
+    <row r="39" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="O39" t="s">
         <v>64</v>
       </c>
-      <c r="O39" t="s">
+      <c r="P39" t="s">
         <v>25</v>
       </c>
-      <c r="R39" t="s">
+      <c r="S39" t="s">
         <v>82</v>
       </c>
-      <c r="S39" t="s">
+      <c r="T39" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="40" spans="14:22" x14ac:dyDescent="0.25">
-      <c r="N40" t="s">
+    <row r="40" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="O40" t="s">
         <v>65</v>
       </c>
-      <c r="O40" t="s">
+      <c r="P40" t="s">
         <v>66</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="G5:G8"/>
-    <mergeCell ref="G16:G18"/>
-    <mergeCell ref="O5:V5"/>
-    <mergeCell ref="X5:AA5"/>
-    <mergeCell ref="P7:U7"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="U28:V28"/>
-    <mergeCell ref="R35:S35"/>
-    <mergeCell ref="R28:S28"/>
-    <mergeCell ref="N25:V26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="V28:W28"/>
+    <mergeCell ref="S35:T35"/>
+    <mergeCell ref="S28:T28"/>
+    <mergeCell ref="O25:W26"/>
+    <mergeCell ref="H5:H8"/>
+    <mergeCell ref="H16:H18"/>
+    <mergeCell ref="P5:W5"/>
+    <mergeCell ref="Y5:AB5"/>
+    <mergeCell ref="Q7:V7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>